<commit_message>
trendline work should be started
</commit_message>
<xml_diff>
--- a/bt_sup_res/tick size.xlsx
+++ b/bt_sup_res/tick size.xlsx
@@ -128,7 +128,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
@@ -199,14 +199,62 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">$A$4*A9</f>
+        <v>666.666666666666</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">$A$4*A10</f>
+        <v>1083.33333333333</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">$A$4*A11</f>
         <v>1666.66666666667</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>1600</v>
+      <c r="C11" s="0" t="n">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">$A$4*A12</f>
+        <v>4166.66666666667</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">$A$4*A13</f>
+        <v>16666.6666666667</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>17000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>